<commit_message>
make a pilot test
</commit_message>
<xml_diff>
--- a/result_group.xlsx
+++ b/result_group.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="42">
   <si>
     <t>Standart AWM</t>
   </si>
@@ -40,88 +40,106 @@
     <t>poi_longitude</t>
   </si>
   <si>
-    <t>Espaco Unibanco de Cinema   Cine Glauber Rocha</t>
-  </si>
-  <si>
-    <t>Sala de Arte Cinema da UFBA</t>
-  </si>
-  <si>
-    <t>Cine XIV</t>
-  </si>
-  <si>
-    <t>UCI Orient Cinemas</t>
-  </si>
-  <si>
-    <t>Museu Geologico da Bahia Sala de Arte Cinema do Museu</t>
-  </si>
-  <si>
-    <t>Cine Paseo</t>
-  </si>
-  <si>
-    <t>Sala Walter da Silveira</t>
-  </si>
-  <si>
-    <t>Cinema do Museu</t>
-  </si>
-  <si>
-    <t>UCI Orient   Shopping da Bahia</t>
-  </si>
-  <si>
-    <t>Orient Shopping Center Lapa</t>
-  </si>
-  <si>
-    <t>cinema</t>
-  </si>
-  <si>
-    <t>NDCG: nan</t>
+    <t>Praia do Farol</t>
+  </si>
+  <si>
+    <t>Muncab - National Museum of Afro Brazilian Culture</t>
+  </si>
+  <si>
+    <t>Praia do Porto da Barra</t>
+  </si>
+  <si>
+    <t>Museum of Brazilian Music</t>
+  </si>
+  <si>
+    <t>Shopping Capemi Salvador</t>
+  </si>
+  <si>
+    <t>Cia Maritima Salvador Shopping</t>
+  </si>
+  <si>
+    <t>Forte de Santo Antonio alem do Carmo</t>
+  </si>
+  <si>
+    <t>Shopping Paralela</t>
+  </si>
+  <si>
+    <t>Ondina Beach</t>
+  </si>
+  <si>
+    <t>Shopping da Bahia</t>
+  </si>
+  <si>
+    <t>beach</t>
+  </si>
+  <si>
+    <t>museum</t>
+  </si>
+  <si>
+    <t>shopping_mall</t>
+  </si>
+  <si>
+    <t>tourist_attraction</t>
+  </si>
+  <si>
+    <t>NDCG: 1.0</t>
   </si>
   <si>
     <t>Diversificado_recs_greedy AWM</t>
   </si>
   <si>
+    <t>CAFETERIA FLORIDA</t>
+  </si>
+  <si>
+    <t>Casa de Cinema da Bahia</t>
+  </si>
+  <si>
+    <t>cafe</t>
+  </si>
+  <si>
+    <t>movie_theater</t>
+  </si>
+  <si>
+    <t>NDCG: 0.9960169407355046</t>
+  </si>
+  <si>
     <t>Diversificado_recs_random AWM</t>
   </si>
   <si>
-    <t>McDonalds</t>
-  </si>
-  <si>
-    <t>Galeria de Arte Paulo Darze</t>
-  </si>
-  <si>
-    <t>Bar da Vila</t>
-  </si>
-  <si>
-    <t>Puro Sabor</t>
-  </si>
-  <si>
-    <t>Caranguejo do Farol</t>
-  </si>
-  <si>
-    <t>Hotel Praia Porto da Barra</t>
-  </si>
-  <si>
-    <t>Barraca Buraco da Velha</t>
-  </si>
-  <si>
-    <t>Amoreiras</t>
-  </si>
-  <si>
-    <t>Praia Jardim de Alah</t>
-  </si>
-  <si>
-    <t>fast_food</t>
-  </si>
-  <si>
-    <t>arts_centre</t>
-  </si>
-  <si>
-    <t>pub</t>
+    <t>Cazolla Gastro Burguer Beer.</t>
+  </si>
+  <si>
+    <t>Bar Lagoa dos Frades</t>
+  </si>
+  <si>
+    <t>Beach Stop</t>
+  </si>
+  <si>
+    <t>Nova Alegria Bar e Restaurante</t>
+  </si>
+  <si>
+    <t>Letreiro Salvador</t>
+  </si>
+  <si>
+    <t>Praia de Stella Maris</t>
+  </si>
+  <si>
+    <t>BaO Petiscaria</t>
+  </si>
+  <si>
+    <t>Praia da Boa Viagem</t>
+  </si>
+  <si>
+    <t>fast-food</t>
+  </si>
+  <si>
+    <t>bar</t>
   </si>
   <si>
     <t>restaurant</t>
   </si>
   <si>
-    <t>Beach</t>
+    <t>NDCG: 0.9247516059377486</t>
   </si>
 </sst>
 </file>
@@ -518,7 +536,7 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>284</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -527,13 +545,16 @@
         <v>18</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>1.581773681253018</v>
+      </c>
+      <c r="F3">
+        <v>0.791</v>
       </c>
       <c r="G3">
-        <v>-12.9771671</v>
+        <v>-12.952961</v>
       </c>
       <c r="H3">
-        <v>-38.5142719</v>
+        <v>-38.348126</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -541,22 +562,25 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>285</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>1.442942753776769</v>
+      </c>
+      <c r="F4">
+        <v>0.746</v>
       </c>
       <c r="G4">
-        <v>-12.9954679</v>
+        <v>-12.9761485</v>
       </c>
       <c r="H4">
-        <v>-38.5187187</v>
+        <v>-38.5124649</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -564,7 +588,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>286</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -573,13 +597,16 @@
         <v>18</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>1.484756941195069</v>
+      </c>
+      <c r="F5">
+        <v>0.742</v>
       </c>
       <c r="G5">
-        <v>-12.9733648</v>
+        <v>-13.0038021</v>
       </c>
       <c r="H5">
-        <v>-38.5080276</v>
+        <v>-38.5326932</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -587,22 +614,25 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>287</v>
+        <v>199</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>1.409365989240249</v>
+      </c>
+      <c r="F6">
+        <v>0.729</v>
       </c>
       <c r="G6">
-        <v>-13.0068948</v>
+        <v>-12.9738253</v>
       </c>
       <c r="H6">
-        <v>-38.52541</v>
+        <v>-38.508487</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -610,22 +640,25 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>288</v>
+        <v>349</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>1.353198932593896</v>
+      </c>
+      <c r="F7">
+        <v>0.714</v>
       </c>
       <c r="G7">
-        <v>-12.9925497</v>
+        <v>-12.9831</v>
       </c>
       <c r="H7">
-        <v>-38.5255217</v>
+        <v>-38.465</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -633,22 +666,25 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>289</v>
+        <v>352</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>1.279649308173254</v>
+      </c>
+      <c r="F8">
+        <v>0.677</v>
       </c>
       <c r="G8">
-        <v>-12.9955106</v>
+        <v>-12.9954162</v>
       </c>
       <c r="H8">
-        <v>-38.4713039</v>
+        <v>-38.4542581</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -656,22 +692,25 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>290</v>
+        <v>378</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>1.33246946639442</v>
+      </c>
+      <c r="F9">
+        <v>0.673</v>
       </c>
       <c r="G9">
-        <v>-12.9857884</v>
+        <v>-12.9636017</v>
       </c>
       <c r="H9">
-        <v>-38.5134954</v>
+        <v>-38.5039186</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -679,22 +718,25 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>291</v>
+        <v>342</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>1.246563807333256</v>
+      </c>
+      <c r="F10">
+        <v>0.661</v>
       </c>
       <c r="G10">
-        <v>-12.9915475</v>
+        <v>-12.9365263</v>
       </c>
       <c r="H10">
-        <v>-38.5252373</v>
+        <v>-38.3949236</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -702,7 +744,7 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>294</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
@@ -711,13 +753,16 @@
         <v>18</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>1.245057115085724</v>
+      </c>
+      <c r="F11">
+        <v>0.66</v>
       </c>
       <c r="G11">
-        <v>-12.982597</v>
+        <v>-13.0103784</v>
       </c>
       <c r="H11">
-        <v>-38.4634301</v>
+        <v>-38.5120368</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -725,32 +770,35 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>295</v>
+        <v>341</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>1.246334170797274</v>
+      </c>
+      <c r="F12">
+        <v>0.66</v>
       </c>
       <c r="G12">
-        <v>-12.9830472</v>
+        <v>-12.9811659</v>
       </c>
       <c r="H12">
-        <v>-38.5137211</v>
+        <v>-38.46503209999999</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -781,7 +829,7 @@
         <v>0</v>
       </c>
       <c r="B17">
-        <v>284</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -790,13 +838,16 @@
         <v>18</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>1.581773681253018</v>
+      </c>
+      <c r="F17">
+        <v>0.791</v>
       </c>
       <c r="G17">
-        <v>-12.9771671</v>
+        <v>-12.952961</v>
       </c>
       <c r="H17">
-        <v>-38.5142719</v>
+        <v>-38.348126</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -804,22 +855,25 @@
         <v>1</v>
       </c>
       <c r="B18">
-        <v>285</v>
+        <v>193</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>1.442942753776769</v>
+      </c>
+      <c r="F18">
+        <v>0.746</v>
       </c>
       <c r="G18">
-        <v>-12.9954679</v>
+        <v>-12.9761485</v>
       </c>
       <c r="H18">
-        <v>-38.5187187</v>
+        <v>-38.5124649</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -827,22 +881,25 @@
         <v>2</v>
       </c>
       <c r="B19">
-        <v>286</v>
+        <v>349</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>1.353198932593896</v>
+      </c>
+      <c r="F19">
+        <v>0.714</v>
       </c>
       <c r="G19">
-        <v>-12.9733648</v>
+        <v>-12.9831</v>
       </c>
       <c r="H19">
-        <v>-38.5080276</v>
+        <v>-38.465</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -850,22 +907,25 @@
         <v>3</v>
       </c>
       <c r="B20">
-        <v>287</v>
+        <v>378</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>1.33246946639442</v>
+      </c>
+      <c r="F20">
+        <v>0.673</v>
       </c>
       <c r="G20">
-        <v>-13.0068948</v>
+        <v>-12.9636017</v>
       </c>
       <c r="H20">
-        <v>-38.52541</v>
+        <v>-38.5039186</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -873,22 +933,25 @@
         <v>4</v>
       </c>
       <c r="B21">
-        <v>288</v>
+        <v>140</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>1.264779587120852</v>
+      </c>
+      <c r="F21">
+        <v>0.654</v>
       </c>
       <c r="G21">
-        <v>-12.9925497</v>
+        <v>-13.0039875</v>
       </c>
       <c r="H21">
-        <v>-38.5255217</v>
+        <v>-38.5023199</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -896,22 +959,25 @@
         <v>5</v>
       </c>
       <c r="B22">
-        <v>289</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
         <v>18</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>1.484756941195069</v>
+      </c>
+      <c r="F22">
+        <v>0.742</v>
       </c>
       <c r="G22">
-        <v>-12.9955106</v>
+        <v>-13.0038021</v>
       </c>
       <c r="H22">
-        <v>-38.4713039</v>
+        <v>-38.5326932</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -919,22 +985,25 @@
         <v>6</v>
       </c>
       <c r="B23">
-        <v>290</v>
+        <v>199</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>1.409365989240249</v>
+      </c>
+      <c r="F23">
+        <v>0.729</v>
       </c>
       <c r="G23">
-        <v>-12.9857884</v>
+        <v>-12.9738253</v>
       </c>
       <c r="H23">
-        <v>-38.5134954</v>
+        <v>-38.508487</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -942,22 +1011,25 @@
         <v>7</v>
       </c>
       <c r="B24">
-        <v>291</v>
+        <v>180</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>1.248761228523516</v>
+      </c>
+      <c r="F24">
+        <v>0.642</v>
       </c>
       <c r="G24">
-        <v>-12.9915475</v>
+        <v>-12.9725511</v>
       </c>
       <c r="H24">
-        <v>-38.5252373</v>
+        <v>-38.508565</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -965,22 +1037,25 @@
         <v>8</v>
       </c>
       <c r="B25">
-        <v>294</v>
+        <v>352</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>1.279649308173254</v>
+      </c>
+      <c r="F25">
+        <v>0.677</v>
       </c>
       <c r="G25">
-        <v>-12.982597</v>
+        <v>-12.9954162</v>
       </c>
       <c r="H25">
-        <v>-38.4634301</v>
+        <v>-38.4542581</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -988,32 +1063,35 @@
         <v>9</v>
       </c>
       <c r="B26">
-        <v>295</v>
+        <v>83</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s">
         <v>18</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>1.245057115085724</v>
+      </c>
+      <c r="F26">
+        <v>0.66</v>
       </c>
       <c r="G26">
-        <v>-12.9830472</v>
+        <v>-13.0103784</v>
       </c>
       <c r="H26">
-        <v>-38.5137211</v>
+        <v>-38.5120368</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1044,25 +1122,25 @@
         <v>0</v>
       </c>
       <c r="B31">
-        <v>406</v>
+        <v>158</v>
       </c>
       <c r="C31" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E31">
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="F31">
-        <v>0.9</v>
+        <v>0.516</v>
       </c>
       <c r="G31">
-        <v>-13.0125695</v>
+        <v>-12.9896638</v>
       </c>
       <c r="H31">
-        <v>-38.4834358</v>
+        <v>-38.4596392</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1070,25 +1148,25 @@
         <v>1</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>0.526</v>
       </c>
       <c r="G32">
-        <v>-12.9950602</v>
+        <v>-12.9807799</v>
       </c>
       <c r="H32">
-        <v>-38.5276959</v>
+        <v>-38.4436399</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1096,22 +1174,25 @@
         <v>2</v>
       </c>
       <c r="B33">
-        <v>287</v>
+        <v>87</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D33" t="s">
         <v>18</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>1.581773681253018</v>
+      </c>
+      <c r="F33">
+        <v>0.791</v>
       </c>
       <c r="G33">
-        <v>-13.0068948</v>
+        <v>-12.952961</v>
       </c>
       <c r="H33">
-        <v>-38.52541</v>
+        <v>-38.348126</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1119,25 +1200,25 @@
         <v>3</v>
       </c>
       <c r="B34">
-        <v>790</v>
+        <v>266</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E34">
-        <v>0.08904541703813904</v>
+        <v>1</v>
       </c>
       <c r="F34">
-        <v>0.045</v>
+        <v>0.528</v>
       </c>
       <c r="G34">
-        <v>-13.0131667</v>
+        <v>-12.932848</v>
       </c>
       <c r="H34">
-        <v>-38.4856513</v>
+        <v>-38.3287828</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1145,25 +1226,25 @@
         <v>4</v>
       </c>
       <c r="B35">
-        <v>826</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
       <c r="F35">
-        <v>0.5</v>
+        <v>0.517</v>
       </c>
       <c r="G35">
-        <v>-13.0105023</v>
+        <v>-12.9693386</v>
       </c>
       <c r="H35">
-        <v>-38.4680809</v>
+        <v>-38.437136</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1171,25 +1252,25 @@
         <v>5</v>
       </c>
       <c r="B36">
-        <v>842</v>
+        <v>377</v>
       </c>
       <c r="C36" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>0.1221469833687715</v>
       </c>
       <c r="F36">
-        <v>0.5</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="G36">
-        <v>-13.0097114</v>
+        <v>-12.974585</v>
       </c>
       <c r="H36">
-        <v>-38.5301932</v>
+        <v>-38.5127509</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1197,22 +1278,25 @@
         <v>6</v>
       </c>
       <c r="B37">
-        <v>1035</v>
+        <v>140</v>
       </c>
       <c r="C37" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D37" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E37">
-        <v>0.5481261541783785</v>
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>0.5</v>
       </c>
       <c r="G37">
-        <v>-13.0044196</v>
+        <v>-13.0039875</v>
       </c>
       <c r="H37">
-        <v>-38.5330276</v>
+        <v>-38.5023199</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1220,22 +1304,25 @@
         <v>7</v>
       </c>
       <c r="B38">
-        <v>1295</v>
+        <v>96</v>
       </c>
       <c r="C38" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D38" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>1.145291351242065</v>
+      </c>
+      <c r="F38">
+        <v>0.573</v>
       </c>
       <c r="G38">
-        <v>-12.8962939887605</v>
+        <v>-12.9488167</v>
       </c>
       <c r="H38">
-        <v>-38.29357072160442</v>
+        <v>-38.341097</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1243,25 +1330,25 @@
         <v>8</v>
       </c>
       <c r="B39">
-        <v>1281</v>
+        <v>60</v>
       </c>
       <c r="C39" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D39" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
       <c r="F39">
-        <v>0.5</v>
+        <v>0.517</v>
       </c>
       <c r="G39">
-        <v>-12.90260172858285</v>
+        <v>-12.97853</v>
       </c>
       <c r="H39">
-        <v>-38.65070813354239</v>
+        <v>-38.4450989</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1269,30 +1356,30 @@
         <v>9</v>
       </c>
       <c r="B40">
-        <v>1278</v>
+        <v>93</v>
       </c>
       <c r="C40" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D40" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>1.129106459124083</v>
       </c>
       <c r="F40">
-        <v>0.5</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="G40">
-        <v>-12.99472635644033</v>
+        <v>-12.9350958</v>
       </c>
       <c r="H40">
-        <v>-38.44260633894478</v>
+        <v>-38.5098867</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
escondendo a chave API
</commit_message>
<xml_diff>
--- a/result_group.xlsx
+++ b/result_group.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="43">
   <si>
     <t>Standart AWM</t>
   </si>
@@ -106,40 +106,43 @@
     <t>Diversificado_recs_random AWM</t>
   </si>
   <si>
-    <t>Cazolla Gastro Burguer Beer.</t>
-  </si>
-  <si>
-    <t>Bar Lagoa dos Frades</t>
-  </si>
-  <si>
-    <t>Beach Stop</t>
-  </si>
-  <si>
-    <t>Nova Alegria Bar e Restaurante</t>
-  </si>
-  <si>
-    <t>Letreiro Salvador</t>
-  </si>
-  <si>
-    <t>Praia de Stella Maris</t>
-  </si>
-  <si>
-    <t>BaO Petiscaria</t>
-  </si>
-  <si>
-    <t>Praia da Boa Viagem</t>
-  </si>
-  <si>
-    <t>fast-food</t>
+    <t>Sal Marinho</t>
+  </si>
+  <si>
+    <t>Bar e Restaurante</t>
+  </si>
+  <si>
+    <t>Ponta do Humaita</t>
+  </si>
+  <si>
+    <t>Praia Pedra do Sal</t>
+  </si>
+  <si>
+    <t>Sentollas Bar e Restaurante</t>
+  </si>
+  <si>
+    <t>Rua 15 Restaurante e Bar</t>
+  </si>
+  <si>
+    <t>Galeria Canizares UFBA</t>
+  </si>
+  <si>
+    <t>Praia de Placafor</t>
+  </si>
+  <si>
+    <t>Praia de Piata</t>
+  </si>
+  <si>
+    <t>Beckels Pizza</t>
   </si>
   <si>
     <t>bar</t>
   </si>
   <si>
-    <t>restaurant</t>
-  </si>
-  <si>
-    <t>NDCG: 0.9247516059377486</t>
+    <t>art_gallery</t>
+  </si>
+  <si>
+    <t>NDCG: 0.9570643210427647</t>
   </si>
 </sst>
 </file>
@@ -1122,25 +1125,25 @@
         <v>0</v>
       </c>
       <c r="B31">
-        <v>158</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E31">
         <v>1</v>
       </c>
       <c r="F31">
-        <v>0.516</v>
+        <v>0.526</v>
       </c>
       <c r="G31">
-        <v>-12.9896638</v>
+        <v>-12.999919</v>
       </c>
       <c r="H31">
-        <v>-38.4596392</v>
+        <v>-38.456829</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1148,25 +1151,25 @@
         <v>1</v>
       </c>
       <c r="B32">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
       <c r="F32">
-        <v>0.526</v>
+        <v>0.517</v>
       </c>
       <c r="G32">
-        <v>-12.9807799</v>
+        <v>-12.9125452</v>
       </c>
       <c r="H32">
-        <v>-38.4436399</v>
+        <v>-38.4971898</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1174,25 +1177,25 @@
         <v>2</v>
       </c>
       <c r="B33">
-        <v>87</v>
+        <v>367</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D33" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E33">
-        <v>1.581773681253018</v>
+        <v>1</v>
       </c>
       <c r="F33">
-        <v>0.791</v>
+        <v>0.507</v>
       </c>
       <c r="G33">
-        <v>-12.952961</v>
+        <v>-12.9299294</v>
       </c>
       <c r="H33">
-        <v>-38.348126</v>
+        <v>-38.5351303</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1200,25 +1203,25 @@
         <v>3</v>
       </c>
       <c r="B34">
-        <v>266</v>
+        <v>111</v>
       </c>
       <c r="C34" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D34" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>1.146865557795592</v>
       </c>
       <c r="F34">
-        <v>0.528</v>
+        <v>0.573</v>
       </c>
       <c r="G34">
-        <v>-12.932848</v>
+        <v>-12.9524313</v>
       </c>
       <c r="H34">
-        <v>-38.3287828</v>
+        <v>-38.3460781</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1226,25 +1229,25 @@
         <v>4</v>
       </c>
       <c r="B35">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C35" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>1.127132897628926</v>
       </c>
       <c r="F35">
-        <v>0.517</v>
+        <v>0.5639999999999999</v>
       </c>
       <c r="G35">
-        <v>-12.9693386</v>
+        <v>-12.967751</v>
       </c>
       <c r="H35">
-        <v>-38.437136</v>
+        <v>-38.4082736</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1252,25 +1255,25 @@
         <v>5</v>
       </c>
       <c r="B36">
-        <v>377</v>
+        <v>47</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D36" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="E36">
-        <v>0.1221469833687715</v>
+        <v>1</v>
       </c>
       <c r="F36">
-        <v>0.08699999999999999</v>
+        <v>0.517</v>
       </c>
       <c r="G36">
-        <v>-12.974585</v>
+        <v>-12.9795299</v>
       </c>
       <c r="H36">
-        <v>-38.5127509</v>
+        <v>-38.4299455</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1278,25 +1281,25 @@
         <v>6</v>
       </c>
       <c r="B37">
-        <v>140</v>
+        <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37">
-        <v>0.5</v>
+        <v>0.016</v>
       </c>
       <c r="G37">
-        <v>-13.0039875</v>
+        <v>-12.9911905</v>
       </c>
       <c r="H37">
-        <v>-38.5023199</v>
+        <v>-38.5211528</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1304,25 +1307,25 @@
         <v>7</v>
       </c>
       <c r="B38">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C38" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D38" t="s">
         <v>18</v>
       </c>
       <c r="E38">
-        <v>1.145291351242065</v>
+        <v>1.219282701737286</v>
       </c>
       <c r="F38">
-        <v>0.573</v>
+        <v>0.61</v>
       </c>
       <c r="G38">
-        <v>-12.9488167</v>
+        <v>-12.9512414</v>
       </c>
       <c r="H38">
-        <v>-38.341097</v>
+        <v>-38.371031</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1330,25 +1333,25 @@
         <v>8</v>
       </c>
       <c r="B39">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D39" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
       <c r="F39">
-        <v>0.517</v>
+        <v>0.538</v>
       </c>
       <c r="G39">
-        <v>-12.97853</v>
+        <v>-12.9547946</v>
       </c>
       <c r="H39">
-        <v>-38.4450989</v>
+        <v>-38.3826836</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1356,30 +1359,30 @@
         <v>9</v>
       </c>
       <c r="B40">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="C40" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D40" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="E40">
-        <v>1.129106459124083</v>
+        <v>1</v>
       </c>
       <c r="F40">
-        <v>0.5649999999999999</v>
+        <v>0.517</v>
       </c>
       <c r="G40">
-        <v>-12.9350958</v>
+        <v>-12.9919109</v>
       </c>
       <c r="H40">
-        <v>-38.5098867</v>
+        <v>-38.4551933</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>